<commit_message>
tz: update sch sth forms
</commit_message>
<xml_diff>
--- a/SCH-STH/Impact assessments/Tanzania/2024/tz_sch_sth_impact_202405_1_school.xlsx
+++ b/SCH-STH/Impact assessments/Tanzania/2024/tz_sch_sth_impact_202405_1_school.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Tanzania\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\SCH-STH\Impact assessments\Tanzania\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F3F345-B2AF-4FAC-B787-8090DA4D3B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E53D1BD6-A195-4C90-8036-48796A47C491}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -2042,10 +2042,10 @@
     <t>Mtazamaji: Ni vifaa gani vya kunawia mikono vinapatikana angalau mita 3 kutoka kwenye vyoo?</t>
   </si>
   <si>
-    <t>(2024 Jan) - 1. SCH/STH – School/Location V4.1</t>
-  </si>
-  <si>
-    <t>tz_sch_sth_impact_202311_1_school_v4_1</t>
+    <t>tz_sch_sth_impact_2405_1_school</t>
+  </si>
+  <si>
+    <t>(2024 May) - 1. SCH/STH – School/Location</t>
   </si>
 </sst>
 </file>
@@ -2253,7 +2253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2325,9 +2325,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2349,7 +2346,7 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2781,8 +2778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D29" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="B29" sqref="B29"/>
@@ -2865,10 +2862,10 @@
       <c r="D2" s="27" t="s">
         <v>391</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="34" t="s">
         <v>399</v>
       </c>
-      <c r="F2" s="35" t="s">
+      <c r="F2" s="34" t="s">
         <v>400</v>
       </c>
       <c r="G2" s="25"/>
@@ -2878,7 +2875,7 @@
       <c r="I2" s="27" t="s">
         <v>365</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="34" t="s">
         <v>407</v>
       </c>
       <c r="K2" s="25"/>
@@ -2900,21 +2897,20 @@
         <v>356</v>
       </c>
       <c r="D3" s="27"/>
-      <c r="E3" s="35" t="s">
+      <c r="E3" s="34" t="s">
         <v>401</v>
       </c>
-      <c r="F3" s="35"/>
+      <c r="F3" s="34"/>
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
       <c r="I3" s="27"/>
-      <c r="J3" s="35"/>
+      <c r="J3" s="34"/>
       <c r="K3" s="25"/>
       <c r="L3" s="25"/>
       <c r="M3" s="25" t="s">
         <v>10</v>
       </c>
       <c r="N3" s="25"/>
-      <c r="O3" s="29"/>
     </row>
     <row r="4" spans="1:15" s="28" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="25" t="s">
@@ -2927,14 +2923,14 @@
         <v>385</v>
       </c>
       <c r="D4" s="27"/>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="34" t="s">
         <v>402</v>
       </c>
-      <c r="F4" s="35"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="25"/>
-      <c r="H4" s="30"/>
+      <c r="H4" s="29"/>
       <c r="I4" s="27"/>
-      <c r="J4" s="35"/>
+      <c r="J4" s="34"/>
       <c r="K4" s="25"/>
       <c r="L4" s="25"/>
       <c r="M4" s="25" t="s">
@@ -2956,14 +2952,14 @@
         <v>386</v>
       </c>
       <c r="D5" s="27"/>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="34" t="s">
         <v>608</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="34"/>
       <c r="G5" s="25"/>
-      <c r="H5" s="30"/>
+      <c r="H5" s="29"/>
       <c r="I5" s="27"/>
-      <c r="J5" s="35"/>
+      <c r="J5" s="34"/>
       <c r="K5" s="25"/>
       <c r="L5" s="25"/>
       <c r="M5" s="25" t="s">
@@ -2985,21 +2981,21 @@
         <v>357</v>
       </c>
       <c r="D6" s="27"/>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="34" t="s">
         <v>403</v>
       </c>
-      <c r="F6" s="35"/>
+      <c r="F6" s="34"/>
       <c r="G6" s="25"/>
       <c r="H6" s="25"/>
       <c r="I6" s="27"/>
-      <c r="J6" s="35"/>
+      <c r="J6" s="34"/>
       <c r="K6" s="25"/>
       <c r="L6" s="25"/>
       <c r="M6" s="25" t="s">
         <v>10</v>
       </c>
       <c r="N6" s="25"/>
-      <c r="O6" s="31" t="s">
+      <c r="O6" s="30" t="s">
         <v>370</v>
       </c>
     </row>
@@ -3014,21 +3010,21 @@
         <v>387</v>
       </c>
       <c r="D7" s="27"/>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="34" t="s">
         <v>404</v>
       </c>
-      <c r="F7" s="35"/>
+      <c r="F7" s="34"/>
       <c r="G7" s="25"/>
       <c r="H7" s="25"/>
       <c r="I7" s="27"/>
-      <c r="J7" s="35"/>
+      <c r="J7" s="34"/>
       <c r="K7" s="25"/>
       <c r="L7" s="25"/>
       <c r="M7" s="25" t="s">
         <v>10</v>
       </c>
       <c r="N7" s="25"/>
-      <c r="O7" s="31" t="s">
+      <c r="O7" s="30" t="s">
         <v>384</v>
       </c>
     </row>
@@ -3045,16 +3041,16 @@
       <c r="D8" s="27" t="s">
         <v>371</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="34" t="s">
         <v>405</v>
       </c>
-      <c r="F8" s="35" t="s">
+      <c r="F8" s="34" t="s">
         <v>406</v>
       </c>
       <c r="G8" s="25"/>
       <c r="H8" s="25"/>
       <c r="I8" s="27"/>
-      <c r="J8" s="35"/>
+      <c r="J8" s="34"/>
       <c r="K8" s="25"/>
       <c r="L8" s="25"/>
       <c r="M8" s="25" t="s">
@@ -3074,14 +3070,14 @@
         <v>609</v>
       </c>
       <c r="D9" s="27"/>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="34" t="s">
         <v>610</v>
       </c>
-      <c r="F9" s="35"/>
+      <c r="F9" s="34"/>
       <c r="G9" s="25"/>
       <c r="H9" s="25"/>
       <c r="I9" s="27"/>
-      <c r="J9" s="35"/>
+      <c r="J9" s="34"/>
       <c r="K9" s="25"/>
       <c r="L9" s="25"/>
       <c r="M9" s="25" t="s">
@@ -3101,14 +3097,14 @@
         <v>611</v>
       </c>
       <c r="D10" s="27"/>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="34" t="s">
         <v>602</v>
       </c>
-      <c r="F10" s="35"/>
+      <c r="F10" s="34"/>
       <c r="G10" s="25"/>
       <c r="H10" s="25"/>
       <c r="I10" s="27"/>
-      <c r="J10" s="35"/>
+      <c r="J10" s="34"/>
       <c r="K10" s="25" t="s">
         <v>621</v>
       </c>
@@ -3132,10 +3128,10 @@
       <c r="D11" s="27" t="s">
         <v>613</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="34" t="s">
         <v>603</v>
       </c>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="34" t="s">
         <v>614</v>
       </c>
       <c r="G11" s="25"/>
@@ -3145,7 +3141,7 @@
       <c r="I11" s="27" t="s">
         <v>595</v>
       </c>
-      <c r="J11" s="35" t="s">
+      <c r="J11" s="34" t="s">
         <v>596</v>
       </c>
       <c r="K11" s="25" t="s">
@@ -3171,16 +3167,16 @@
       <c r="D12" s="27" t="s">
         <v>604</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="34" t="s">
         <v>409</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="34" t="s">
         <v>410</v>
       </c>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
       <c r="I12" s="27"/>
-      <c r="J12" s="35"/>
+      <c r="J12" s="34"/>
       <c r="K12" s="25" t="s">
         <v>621</v>
       </c>
@@ -3204,16 +3200,16 @@
       <c r="D13" s="27" t="s">
         <v>604</v>
       </c>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="34" t="s">
         <v>412</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="34" t="s">
         <v>410</v>
       </c>
       <c r="G13" s="25"/>
       <c r="H13" s="25"/>
       <c r="I13" s="27"/>
-      <c r="J13" s="35"/>
+      <c r="J13" s="34"/>
       <c r="K13" s="25" t="s">
         <v>621</v>
       </c>
@@ -3237,16 +3233,16 @@
       <c r="D14" s="27" t="s">
         <v>604</v>
       </c>
-      <c r="E14" s="35" t="s">
+      <c r="E14" s="34" t="s">
         <v>414</v>
       </c>
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="34" t="s">
         <v>410</v>
       </c>
       <c r="G14" s="25"/>
       <c r="H14" s="25"/>
       <c r="I14" s="27"/>
-      <c r="J14" s="35"/>
+      <c r="J14" s="34"/>
       <c r="K14" s="25" t="s">
         <v>621</v>
       </c>
@@ -3270,10 +3266,10 @@
       <c r="D15" s="27" t="s">
         <v>416</v>
       </c>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="34" t="s">
         <v>417</v>
       </c>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="34" t="s">
         <v>418</v>
       </c>
       <c r="G15" s="25"/>
@@ -3283,7 +3279,7 @@
       <c r="I15" s="27" t="s">
         <v>419</v>
       </c>
-      <c r="J15" s="35" t="s">
+      <c r="J15" s="34" t="s">
         <v>420</v>
       </c>
       <c r="K15" s="25" t="s">
@@ -3309,10 +3305,10 @@
       <c r="D16" s="27" t="s">
         <v>416</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="34" t="s">
         <v>422</v>
       </c>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="34" t="s">
         <v>418</v>
       </c>
       <c r="G16" s="25"/>
@@ -3322,7 +3318,7 @@
       <c r="I16" s="27" t="s">
         <v>423</v>
       </c>
-      <c r="J16" s="35" t="s">
+      <c r="J16" s="34" t="s">
         <v>424</v>
       </c>
       <c r="K16" s="25" t="s">
@@ -3348,10 +3344,10 @@
       <c r="D17" s="27" t="s">
         <v>416</v>
       </c>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="34" t="s">
         <v>426</v>
       </c>
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="34" t="s">
         <v>418</v>
       </c>
       <c r="G17" s="25"/>
@@ -3361,7 +3357,7 @@
       <c r="I17" s="27" t="s">
         <v>427</v>
       </c>
-      <c r="J17" s="35" t="s">
+      <c r="J17" s="34" t="s">
         <v>428</v>
       </c>
       <c r="K17" s="25" t="s">
@@ -3385,14 +3381,14 @@
         <v>623</v>
       </c>
       <c r="D18" s="27"/>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="34" t="s">
         <v>622</v>
       </c>
-      <c r="F18" s="35"/>
+      <c r="F18" s="34"/>
       <c r="G18" s="25"/>
       <c r="H18" s="25"/>
       <c r="I18" s="27"/>
-      <c r="J18" s="35"/>
+      <c r="J18" s="34"/>
       <c r="K18" s="25" t="s">
         <v>621</v>
       </c>
@@ -3414,14 +3410,14 @@
         <v>432</v>
       </c>
       <c r="D19" s="27"/>
-      <c r="E19" s="35" t="s">
+      <c r="E19" s="34" t="s">
         <v>433</v>
       </c>
-      <c r="F19" s="35"/>
+      <c r="F19" s="34"/>
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
       <c r="I19" s="27"/>
-      <c r="J19" s="35"/>
+      <c r="J19" s="34"/>
       <c r="K19" s="25" t="s">
         <v>621</v>
       </c>
@@ -3445,16 +3441,16 @@
       <c r="D20" s="27" t="s">
         <v>436</v>
       </c>
-      <c r="E20" s="35" t="s">
+      <c r="E20" s="34" t="s">
         <v>437</v>
       </c>
-      <c r="F20" s="35" t="s">
+      <c r="F20" s="34" t="s">
         <v>438</v>
       </c>
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
       <c r="I20" s="27"/>
-      <c r="J20" s="35"/>
+      <c r="J20" s="34"/>
       <c r="K20" s="25" t="s">
         <v>629</v>
       </c>
@@ -3478,16 +3474,16 @@
       <c r="D21" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="E21" s="35" t="s">
+      <c r="E21" s="34" t="s">
         <v>635</v>
       </c>
-      <c r="F21" s="35" t="s">
+      <c r="F21" s="34" t="s">
         <v>636</v>
       </c>
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
       <c r="I21" s="27"/>
-      <c r="J21" s="35"/>
+      <c r="J21" s="34"/>
       <c r="K21" s="25" t="s">
         <v>621</v>
       </c>
@@ -3509,14 +3505,14 @@
         <v>442</v>
       </c>
       <c r="D22" s="27"/>
-      <c r="E22" s="35" t="s">
+      <c r="E22" s="34" t="s">
         <v>443</v>
       </c>
-      <c r="F22" s="35"/>
+      <c r="F22" s="34"/>
       <c r="G22" s="25"/>
       <c r="H22" s="25"/>
       <c r="I22" s="27"/>
-      <c r="J22" s="35"/>
+      <c r="J22" s="34"/>
       <c r="K22" s="25" t="s">
         <v>621</v>
       </c>
@@ -3540,14 +3536,14 @@
       <c r="D23" s="27" t="s">
         <v>436</v>
       </c>
-      <c r="E23" s="35" t="s">
+      <c r="E23" s="34" t="s">
         <v>446</v>
       </c>
-      <c r="F23" s="35"/>
+      <c r="F23" s="34"/>
       <c r="G23" s="25"/>
       <c r="H23" s="25"/>
       <c r="I23" s="27"/>
-      <c r="J23" s="35"/>
+      <c r="J23" s="34"/>
       <c r="K23" s="25" t="s">
         <v>630</v>
       </c>
@@ -3571,16 +3567,16 @@
       <c r="D24" s="27" t="s">
         <v>440</v>
       </c>
-      <c r="E24" s="65" t="s">
+      <c r="E24" s="64" t="s">
         <v>646</v>
       </c>
-      <c r="F24" s="35" t="s">
+      <c r="F24" s="34" t="s">
         <v>636</v>
       </c>
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
       <c r="I24" s="27"/>
-      <c r="J24" s="35"/>
+      <c r="J24" s="34"/>
       <c r="K24" s="25" t="s">
         <v>621</v>
       </c>
@@ -3604,16 +3600,16 @@
       <c r="D25" s="27" t="s">
         <v>372</v>
       </c>
-      <c r="E25" s="35" t="s">
+      <c r="E25" s="34" t="s">
         <v>457</v>
       </c>
-      <c r="F25" s="35" t="s">
+      <c r="F25" s="34" t="s">
         <v>458</v>
       </c>
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
       <c r="I25" s="27"/>
-      <c r="J25" s="35"/>
+      <c r="J25" s="34"/>
       <c r="K25" s="25" t="s">
         <v>621</v>
       </c>
@@ -3631,31 +3627,31 @@
       <c r="B26" s="26" t="s">
         <v>460</v>
       </c>
-      <c r="C26" s="32" t="s">
+      <c r="C26" s="31" t="s">
         <v>461</v>
       </c>
-      <c r="D26" s="32" t="s">
+      <c r="D26" s="31" t="s">
         <v>462</v>
       </c>
-      <c r="E26" s="36" t="s">
+      <c r="E26" s="35" t="s">
         <v>640</v>
       </c>
-      <c r="F26" s="36" t="s">
+      <c r="F26" s="35" t="s">
         <v>463</v>
       </c>
-      <c r="G26" s="33"/>
-      <c r="H26" s="33"/>
-      <c r="I26" s="32"/>
-      <c r="J26" s="36"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="31"/>
+      <c r="J26" s="35"/>
       <c r="K26" s="25" t="s">
         <v>641</v>
       </c>
-      <c r="L26" s="33"/>
+      <c r="L26" s="32"/>
       <c r="M26" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="N26" s="33"/>
-      <c r="O26" s="33"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
     </row>
     <row r="27" spans="1:15" s="14" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
@@ -3664,31 +3660,31 @@
       <c r="B27" s="26" t="s">
         <v>464</v>
       </c>
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="31" t="s">
         <v>465</v>
       </c>
-      <c r="D27" s="32" t="s">
+      <c r="D27" s="31" t="s">
         <v>436</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="35" t="s">
         <v>466</v>
       </c>
-      <c r="F27" s="36" t="s">
+      <c r="F27" s="35" t="s">
         <v>438</v>
       </c>
-      <c r="G27" s="33"/>
-      <c r="H27" s="33"/>
-      <c r="I27" s="32"/>
-      <c r="J27" s="36"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="35"/>
       <c r="K27" s="25" t="s">
         <v>631</v>
       </c>
-      <c r="L27" s="33"/>
+      <c r="L27" s="32"/>
       <c r="M27" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="N27" s="33"/>
-      <c r="O27" s="33"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
     </row>
     <row r="28" spans="1:15" s="14" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
@@ -3697,27 +3693,27 @@
       <c r="B28" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="31" t="s">
         <v>467</v>
       </c>
-      <c r="D28" s="32"/>
-      <c r="E28" s="36" t="s">
+      <c r="D28" s="31"/>
+      <c r="E28" s="35" t="s">
         <v>468</v>
       </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="33"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="32"/>
-      <c r="J28" s="36"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="31"/>
+      <c r="J28" s="35"/>
       <c r="K28" s="25" t="s">
         <v>632</v>
       </c>
-      <c r="L28" s="33"/>
+      <c r="L28" s="32"/>
       <c r="M28" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
     </row>
     <row r="29" spans="1:15" s="28" customFormat="1" ht="63" x14ac:dyDescent="0.25">
       <c r="A29" s="25" t="s">
@@ -3732,16 +3728,16 @@
       <c r="D29" s="27" t="s">
         <v>605</v>
       </c>
-      <c r="E29" s="35" t="s">
+      <c r="E29" s="34" t="s">
         <v>471</v>
       </c>
-      <c r="F29" s="35" t="s">
+      <c r="F29" s="34" t="s">
         <v>472</v>
       </c>
       <c r="G29" s="25"/>
       <c r="H29" s="25"/>
       <c r="I29" s="27"/>
-      <c r="J29" s="35"/>
+      <c r="J29" s="34"/>
       <c r="K29" s="25" t="s">
         <v>633</v>
       </c>
@@ -3763,14 +3759,14 @@
         <v>359</v>
       </c>
       <c r="D30" s="27"/>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="34" t="s">
         <v>616</v>
       </c>
-      <c r="F30" s="35"/>
+      <c r="F30" s="34"/>
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
       <c r="I30" s="27"/>
-      <c r="J30" s="35"/>
+      <c r="J30" s="34"/>
       <c r="K30" s="25" t="s">
         <v>632</v>
       </c>
@@ -3788,31 +3784,31 @@
       <c r="B31" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="31" t="s">
         <v>360</v>
       </c>
       <c r="D31" s="27" t="s">
         <v>373</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="34" t="s">
         <v>617</v>
       </c>
-      <c r="F31" s="35" t="s">
+      <c r="F31" s="34" t="s">
         <v>618</v>
       </c>
-      <c r="G31" s="33"/>
-      <c r="H31" s="33"/>
-      <c r="I31" s="32"/>
-      <c r="J31" s="36"/>
+      <c r="G31" s="32"/>
+      <c r="H31" s="32"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="35"/>
       <c r="K31" s="25" t="s">
         <v>632</v>
       </c>
-      <c r="L31" s="33"/>
+      <c r="L31" s="32"/>
       <c r="M31" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="N31" s="33"/>
-      <c r="O31" s="33"/>
+      <c r="N31" s="32"/>
+      <c r="O31" s="32"/>
     </row>
     <row r="32" spans="1:15" s="14" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
@@ -3821,31 +3817,31 @@
       <c r="B32" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C32" s="32" t="s">
+      <c r="C32" s="31" t="s">
         <v>361</v>
       </c>
       <c r="D32" s="27" t="s">
         <v>374</v>
       </c>
-      <c r="E32" s="65" t="s">
+      <c r="E32" s="64" t="s">
         <v>647</v>
       </c>
-      <c r="F32" s="35" t="s">
+      <c r="F32" s="34" t="s">
         <v>619</v>
       </c>
-      <c r="G32" s="33"/>
-      <c r="H32" s="33"/>
-      <c r="I32" s="32"/>
-      <c r="J32" s="36"/>
+      <c r="G32" s="32"/>
+      <c r="H32" s="32"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="35"/>
       <c r="K32" s="25" t="s">
         <v>632</v>
       </c>
-      <c r="L32" s="33"/>
+      <c r="L32" s="32"/>
       <c r="M32" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="N32" s="33"/>
-      <c r="O32" s="33"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
     </row>
     <row r="33" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="25" t="s">
@@ -3854,23 +3850,23 @@
       <c r="B33" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C33" s="32" t="s">
+      <c r="C33" s="31" t="s">
         <v>362</v>
       </c>
-      <c r="D33" s="32"/>
-      <c r="E33" s="36" t="s">
+      <c r="D33" s="31"/>
+      <c r="E33" s="35" t="s">
         <v>620</v>
       </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="33"/>
-      <c r="H33" s="33"/>
-      <c r="I33" s="32"/>
-      <c r="J33" s="37"/>
+      <c r="F33" s="35"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="36"/>
       <c r="K33" s="12"/>
-      <c r="L33" s="33"/>
+      <c r="L33" s="32"/>
       <c r="M33" s="25"/>
-      <c r="N33" s="33"/>
-      <c r="O33" s="33"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
     </row>
     <row r="34" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="25" t="s">
@@ -3879,19 +3875,19 @@
       <c r="B34" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="32"/>
-      <c r="D34" s="32"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="32"/>
-      <c r="J34" s="37"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="35"/>
+      <c r="F34" s="35"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="36"/>
       <c r="K34" s="12"/>
-      <c r="L34" s="33"/>
+      <c r="L34" s="32"/>
       <c r="M34" s="25"/>
-      <c r="N34" s="33"/>
-      <c r="O34" s="33"/>
+      <c r="N34" s="32"/>
+      <c r="O34" s="32"/>
     </row>
     <row r="35" spans="1:15" s="14" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
@@ -3900,19 +3896,19 @@
       <c r="B35" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="36"/>
-      <c r="F35" s="36"/>
-      <c r="G35" s="33"/>
-      <c r="H35" s="33"/>
-      <c r="I35" s="32"/>
-      <c r="J35" s="37"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="35"/>
+      <c r="F35" s="35"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="36"/>
       <c r="K35" s="12"/>
-      <c r="L35" s="33"/>
+      <c r="L35" s="32"/>
       <c r="M35" s="25"/>
-      <c r="N35" s="33"/>
-      <c r="O35" s="33"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3925,7 +3921,7 @@
   <dimension ref="A1:H565"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A87" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -3942,28 +3938,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39" t="s">
+      <c r="C1" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="39" t="s">
+      <c r="D1" s="38" t="s">
         <v>396</v>
       </c>
-      <c r="E1" s="39" t="s">
+      <c r="E1" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="G1" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="40" t="s">
         <v>353</v>
       </c>
     </row>
@@ -3977,7 +3973,7 @@
       <c r="C2" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="41" t="s">
         <v>473</v>
       </c>
       <c r="E2" s="5"/>
@@ -3994,7 +3990,7 @@
       <c r="C3" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D3" s="42" t="s">
+      <c r="D3" s="41" t="s">
         <v>474</v>
       </c>
       <c r="E3" s="5"/>
@@ -4011,7 +4007,7 @@
       <c r="C4" s="5" t="s">
         <v>334</v>
       </c>
-      <c r="D4" s="42" t="s">
+      <c r="D4" s="41" t="s">
         <v>473</v>
       </c>
       <c r="E4" s="5"/>
@@ -4028,7 +4024,7 @@
       <c r="C5" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="41" t="s">
         <v>474</v>
       </c>
       <c r="E5" s="5"/>
@@ -4045,7 +4041,7 @@
       <c r="C6" s="5" t="s">
         <v>336</v>
       </c>
-      <c r="D6" s="42" t="s">
+      <c r="D6" s="41" t="s">
         <v>475</v>
       </c>
       <c r="E6" s="5"/>
@@ -4056,22 +4052,22 @@
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
-      <c r="D7" s="42"/>
+      <c r="D7" s="41"/>
       <c r="E7" s="5"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="42" t="s">
+      <c r="A8" s="41" t="s">
         <v>476</v>
       </c>
-      <c r="B8" s="42" t="s">
+      <c r="B8" s="41" t="s">
         <v>477</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="42" t="s">
         <v>478</v>
       </c>
-      <c r="D8" s="42" t="s">
+      <c r="D8" s="41" t="s">
         <v>479</v>
       </c>
       <c r="E8" s="5"/>
@@ -4079,16 +4075,16 @@
       <c r="G8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="42" t="s">
+      <c r="A9" s="41" t="s">
         <v>476</v>
       </c>
-      <c r="B9" s="42" t="s">
+      <c r="B9" s="41" t="s">
         <v>480</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C9" s="42" t="s">
         <v>481</v>
       </c>
-      <c r="D9" s="42" t="s">
+      <c r="D9" s="41" t="s">
         <v>482</v>
       </c>
       <c r="E9" s="5"/>
@@ -4096,16 +4092,16 @@
       <c r="G9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
+      <c r="A10" s="41" t="s">
         <v>476</v>
       </c>
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="41" t="s">
         <v>643</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>643</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="41" t="s">
         <v>642</v>
       </c>
       <c r="E10" s="5"/>
@@ -4113,16 +4109,16 @@
       <c r="G10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="41" t="s">
         <v>476</v>
       </c>
-      <c r="B11" s="42" t="s">
+      <c r="B11" s="41" t="s">
         <v>483</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="C11" s="42" t="s">
         <v>483</v>
       </c>
-      <c r="D11" s="42" t="s">
+      <c r="D11" s="41" t="s">
         <v>484</v>
       </c>
       <c r="E11" s="5"/>
@@ -4130,166 +4126,166 @@
       <c r="G11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="43" t="s">
         <v>485</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="43" t="s">
         <v>343</v>
       </c>
-      <c r="C12" s="45" t="s">
+      <c r="C12" s="44" t="s">
         <v>343</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="45" t="s">
         <v>486</v>
       </c>
-      <c r="E12" s="45"/>
-      <c r="F12" s="47"/>
-      <c r="G12" s="47"/>
-      <c r="H12" s="48"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="47"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="44" t="s">
+      <c r="A13" s="43" t="s">
         <v>485</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="45" t="s">
         <v>336</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="48" t="s">
         <v>336</v>
       </c>
-      <c r="D13" s="46" t="s">
+      <c r="D13" s="45" t="s">
         <v>475</v>
       </c>
-      <c r="E13" s="45"/>
-      <c r="F13" s="47"/>
-      <c r="G13" s="47"/>
-      <c r="H13" s="48"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="47"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="44" t="s">
+      <c r="A14" s="43" t="s">
         <v>485</v>
       </c>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="43" t="s">
         <v>487</v>
       </c>
-      <c r="C14" s="45" t="s">
+      <c r="C14" s="44" t="s">
         <v>487</v>
       </c>
-      <c r="D14" s="46" t="s">
+      <c r="D14" s="45" t="s">
         <v>488</v>
       </c>
-      <c r="E14" s="45"/>
-      <c r="F14" s="47"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="48"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="47"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="44" t="s">
+      <c r="A15" s="43" t="s">
         <v>485</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="43" t="s">
         <v>489</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="44" t="s">
         <v>489</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="45" t="s">
         <v>490</v>
       </c>
-      <c r="E15" s="45"/>
-      <c r="F15" s="47"/>
-      <c r="G15" s="47"/>
-      <c r="H15" s="48"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="47"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="44" t="s">
+      <c r="A16" s="43" t="s">
         <v>485</v>
       </c>
-      <c r="B16" s="44" t="s">
+      <c r="B16" s="43" t="s">
         <v>491</v>
       </c>
-      <c r="C16" s="45" t="s">
+      <c r="C16" s="44" t="s">
         <v>491</v>
       </c>
-      <c r="D16" s="46" t="s">
+      <c r="D16" s="45" t="s">
         <v>492</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="47"/>
-      <c r="G16" s="47"/>
-      <c r="H16" s="48"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="47"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="44" t="s">
+      <c r="A17" s="43" t="s">
         <v>485</v>
       </c>
-      <c r="B17" s="44" t="s">
+      <c r="B17" s="43" t="s">
         <v>493</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="44" t="s">
         <v>493</v>
       </c>
-      <c r="D17" s="46" t="s">
+      <c r="D17" s="45" t="s">
         <v>494</v>
       </c>
-      <c r="E17" s="45"/>
-      <c r="F17" s="47"/>
-      <c r="G17" s="47"/>
-      <c r="H17" s="48"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="47"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="44" t="s">
+      <c r="A18" s="43" t="s">
         <v>485</v>
       </c>
-      <c r="B18" s="44" t="s">
+      <c r="B18" s="43" t="s">
         <v>495</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="44" t="s">
         <v>495</v>
       </c>
-      <c r="D18" s="46" t="s">
+      <c r="D18" s="45" t="s">
         <v>496</v>
       </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="48"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="47"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="44" t="s">
+      <c r="A19" s="43" t="s">
         <v>485</v>
       </c>
-      <c r="B19" s="44" t="s">
+      <c r="B19" s="43" t="s">
         <v>497</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="44" t="s">
         <v>497</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="45" t="s">
         <v>498</v>
       </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="48"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="47"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="44" t="s">
+      <c r="A20" s="43" t="s">
         <v>485</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="43" t="s">
         <v>499</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="44" t="s">
         <v>499</v>
       </c>
-      <c r="D20" s="46" t="s">
+      <c r="D20" s="45" t="s">
         <v>500</v>
       </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="48"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="47"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
@@ -4307,7 +4303,7 @@
       <c r="B22" s="4">
         <v>1</v>
       </c>
-      <c r="C22" s="42" t="s">
+      <c r="C22" s="41" t="s">
         <v>501</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -4324,7 +4320,7 @@
       <c r="B23" s="4">
         <v>2</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="41" t="s">
         <v>502</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -4341,7 +4337,7 @@
       <c r="B24" s="4">
         <v>3</v>
       </c>
-      <c r="C24" s="42" t="s">
+      <c r="C24" s="41" t="s">
         <v>504</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -4358,7 +4354,7 @@
       <c r="B25" s="4">
         <v>4</v>
       </c>
-      <c r="C25" s="42" t="s">
+      <c r="C25" s="41" t="s">
         <v>506</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -4375,7 +4371,7 @@
       <c r="B26" s="4">
         <v>5</v>
       </c>
-      <c r="C26" s="42" t="s">
+      <c r="C26" s="41" t="s">
         <v>508</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -4392,7 +4388,7 @@
       <c r="B27" s="4">
         <v>6</v>
       </c>
-      <c r="C27" s="42" t="s">
+      <c r="C27" s="41" t="s">
         <v>510</v>
       </c>
       <c r="D27" s="4" t="s">
@@ -4409,7 +4405,7 @@
       <c r="B28" s="4">
         <v>7</v>
       </c>
-      <c r="C28" s="42" t="s">
+      <c r="C28" s="41" t="s">
         <v>512</v>
       </c>
       <c r="D28" s="4" t="s">
@@ -4426,7 +4422,7 @@
       <c r="B29" s="4">
         <v>8</v>
       </c>
-      <c r="C29" s="42" t="s">
+      <c r="C29" s="41" t="s">
         <v>514</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -4443,7 +4439,7 @@
       <c r="B30" s="4">
         <v>9</v>
       </c>
-      <c r="C30" s="42" t="s">
+      <c r="C30" s="41" t="s">
         <v>337</v>
       </c>
       <c r="D30" s="4" t="s">
@@ -4460,7 +4456,7 @@
       <c r="B31" s="4">
         <v>10</v>
       </c>
-      <c r="C31" s="42" t="s">
+      <c r="C31" s="41" t="s">
         <v>517</v>
       </c>
       <c r="D31" s="4" t="s">
@@ -4477,7 +4473,7 @@
       <c r="B32" s="4">
         <v>11</v>
       </c>
-      <c r="C32" s="42" t="s">
+      <c r="C32" s="41" t="s">
         <v>519</v>
       </c>
       <c r="D32" s="4" t="s">
@@ -4494,7 +4490,7 @@
       <c r="B33" s="4">
         <v>12</v>
       </c>
-      <c r="C33" s="42" t="s">
+      <c r="C33" s="41" t="s">
         <v>521</v>
       </c>
       <c r="D33" s="4" t="s">
@@ -4511,7 +4507,7 @@
       <c r="B34" s="4">
         <v>13</v>
       </c>
-      <c r="C34" s="42" t="s">
+      <c r="C34" s="41" t="s">
         <v>523</v>
       </c>
       <c r="D34" s="4" t="s">
@@ -4528,7 +4524,7 @@
       <c r="B35" s="4">
         <v>14</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="55" t="s">
         <v>627</v>
       </c>
       <c r="D35" s="2" t="s">
@@ -4542,7 +4538,7 @@
       <c r="B36" s="4">
         <v>66</v>
       </c>
-      <c r="C36" s="42" t="s">
+      <c r="C36" s="41" t="s">
         <v>525</v>
       </c>
       <c r="D36" s="4" t="s">
@@ -4559,7 +4555,7 @@
       <c r="B37" s="4">
         <v>88</v>
       </c>
-      <c r="C37" s="42" t="s">
+      <c r="C37" s="41" t="s">
         <v>628</v>
       </c>
       <c r="D37" s="4" t="s">
@@ -4572,283 +4568,283 @@
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
-      <c r="C38" s="42"/>
+      <c r="C38" s="41"/>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
     </row>
-    <row r="39" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="57" t="s">
+    <row r="39" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B39" s="57">
+      <c r="B39" s="56">
         <v>1</v>
       </c>
-      <c r="C39" s="66" t="s">
+      <c r="C39" s="65" t="s">
         <v>501</v>
       </c>
-      <c r="D39" s="62" t="s">
+      <c r="D39" s="61" t="s">
         <v>625</v>
       </c>
-      <c r="E39" s="57"/>
-      <c r="F39" s="58"/>
-      <c r="G39" s="58"/>
-    </row>
-    <row r="40" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="57" t="s">
+      <c r="E39" s="56"/>
+      <c r="F39" s="57"/>
+      <c r="G39" s="57"/>
+    </row>
+    <row r="40" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B40" s="57">
+      <c r="B40" s="56">
         <v>2</v>
       </c>
-      <c r="C40" s="66" t="s">
+      <c r="C40" s="65" t="s">
         <v>502</v>
       </c>
-      <c r="D40" s="62" t="s">
+      <c r="D40" s="61" t="s">
         <v>503</v>
       </c>
-      <c r="E40" s="57"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="58"/>
-    </row>
-    <row r="41" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="57" t="s">
+      <c r="E40" s="56"/>
+      <c r="F40" s="57"/>
+      <c r="G40" s="57"/>
+    </row>
+    <row r="41" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B41" s="57">
+      <c r="B41" s="56">
         <v>3</v>
       </c>
-      <c r="C41" s="66" t="s">
+      <c r="C41" s="65" t="s">
         <v>504</v>
       </c>
-      <c r="D41" s="62" t="s">
+      <c r="D41" s="61" t="s">
         <v>505</v>
       </c>
-      <c r="E41" s="57"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
-    </row>
-    <row r="42" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="57" t="s">
+      <c r="E41" s="56"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="57"/>
+    </row>
+    <row r="42" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B42" s="57">
+      <c r="B42" s="56">
         <v>4</v>
       </c>
-      <c r="C42" s="66" t="s">
+      <c r="C42" s="65" t="s">
         <v>506</v>
       </c>
-      <c r="D42" s="62" t="s">
+      <c r="D42" s="61" t="s">
         <v>507</v>
       </c>
-      <c r="E42" s="57"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="58"/>
-    </row>
-    <row r="43" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="57" t="s">
+      <c r="E42" s="56"/>
+      <c r="F42" s="57"/>
+      <c r="G42" s="57"/>
+    </row>
+    <row r="43" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B43" s="57">
+      <c r="B43" s="56">
         <v>5</v>
       </c>
-      <c r="C43" s="66" t="s">
+      <c r="C43" s="65" t="s">
         <v>508</v>
       </c>
-      <c r="D43" s="62" t="s">
+      <c r="D43" s="61" t="s">
         <v>509</v>
       </c>
-      <c r="E43" s="57"/>
-      <c r="F43" s="58"/>
-      <c r="G43" s="58"/>
-    </row>
-    <row r="44" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="57" t="s">
+      <c r="E43" s="56"/>
+      <c r="F43" s="57"/>
+      <c r="G43" s="57"/>
+    </row>
+    <row r="44" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B44" s="57">
+      <c r="B44" s="56">
         <v>6</v>
       </c>
-      <c r="C44" s="66" t="s">
+      <c r="C44" s="65" t="s">
         <v>510</v>
       </c>
-      <c r="D44" s="62" t="s">
+      <c r="D44" s="61" t="s">
         <v>511</v>
       </c>
-      <c r="E44" s="57"/>
-      <c r="F44" s="58"/>
-      <c r="G44" s="58"/>
-    </row>
-    <row r="45" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="57" t="s">
+      <c r="E44" s="56"/>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57"/>
+    </row>
+    <row r="45" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B45" s="57">
+      <c r="B45" s="56">
         <v>7</v>
       </c>
-      <c r="C45" s="66" t="s">
+      <c r="C45" s="65" t="s">
         <v>512</v>
       </c>
-      <c r="D45" s="62" t="s">
+      <c r="D45" s="61" t="s">
         <v>513</v>
       </c>
-      <c r="E45" s="57"/>
-      <c r="F45" s="58"/>
-      <c r="G45" s="58"/>
-    </row>
-    <row r="46" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="57" t="s">
+      <c r="E45" s="56"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+    </row>
+    <row r="46" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B46" s="57">
+      <c r="B46" s="56">
         <v>8</v>
       </c>
-      <c r="C46" s="66" t="s">
+      <c r="C46" s="65" t="s">
         <v>514</v>
       </c>
-      <c r="D46" s="62" t="s">
+      <c r="D46" s="61" t="s">
         <v>515</v>
       </c>
-      <c r="E46" s="57"/>
-      <c r="F46" s="58"/>
-      <c r="G46" s="58"/>
-    </row>
-    <row r="47" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="57" t="s">
+      <c r="E46" s="56"/>
+      <c r="F46" s="57"/>
+      <c r="G46" s="57"/>
+    </row>
+    <row r="47" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B47" s="57">
+      <c r="B47" s="56">
         <v>9</v>
       </c>
-      <c r="C47" s="66" t="s">
+      <c r="C47" s="65" t="s">
         <v>337</v>
       </c>
-      <c r="D47" s="62" t="s">
+      <c r="D47" s="61" t="s">
         <v>516</v>
       </c>
-      <c r="E47" s="57"/>
-      <c r="F47" s="58"/>
-      <c r="G47" s="58"/>
-    </row>
-    <row r="48" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="57" t="s">
+      <c r="E47" s="56"/>
+      <c r="F47" s="57"/>
+      <c r="G47" s="57"/>
+    </row>
+    <row r="48" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B48" s="57">
+      <c r="B48" s="56">
         <v>10</v>
       </c>
-      <c r="C48" s="66" t="s">
+      <c r="C48" s="65" t="s">
         <v>517</v>
       </c>
-      <c r="D48" s="62" t="s">
+      <c r="D48" s="61" t="s">
         <v>518</v>
       </c>
-      <c r="E48" s="57"/>
-      <c r="F48" s="58"/>
-      <c r="G48" s="58"/>
-    </row>
-    <row r="49" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="57" t="s">
+      <c r="E48" s="56"/>
+      <c r="F48" s="57"/>
+      <c r="G48" s="57"/>
+    </row>
+    <row r="49" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B49" s="57">
+      <c r="B49" s="56">
         <v>11</v>
       </c>
-      <c r="C49" s="66" t="s">
+      <c r="C49" s="65" t="s">
         <v>519</v>
       </c>
-      <c r="D49" s="62" t="s">
+      <c r="D49" s="61" t="s">
         <v>520</v>
       </c>
-      <c r="E49" s="57"/>
-      <c r="F49" s="58"/>
-      <c r="G49" s="58"/>
-    </row>
-    <row r="50" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="57" t="s">
+      <c r="E49" s="56"/>
+      <c r="F49" s="57"/>
+      <c r="G49" s="57"/>
+    </row>
+    <row r="50" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B50" s="57">
+      <c r="B50" s="56">
         <v>12</v>
       </c>
-      <c r="C50" s="66" t="s">
+      <c r="C50" s="65" t="s">
         <v>521</v>
       </c>
-      <c r="D50" s="62" t="s">
+      <c r="D50" s="61" t="s">
         <v>522</v>
       </c>
-      <c r="E50" s="57"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-    </row>
-    <row r="51" spans="1:7" s="59" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A51" s="57" t="s">
+      <c r="E50" s="56"/>
+      <c r="F50" s="57"/>
+      <c r="G50" s="57"/>
+    </row>
+    <row r="51" spans="1:7" s="58" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B51" s="57">
+      <c r="B51" s="56">
         <v>13</v>
       </c>
-      <c r="C51" s="66" t="s">
+      <c r="C51" s="65" t="s">
         <v>523</v>
       </c>
-      <c r="D51" s="62" t="s">
+      <c r="D51" s="61" t="s">
         <v>524</v>
       </c>
-      <c r="E51" s="57"/>
-      <c r="F51" s="58"/>
-      <c r="G51" s="58"/>
-    </row>
-    <row r="52" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="57" t="s">
+      <c r="E51" s="56"/>
+      <c r="F51" s="57"/>
+      <c r="G51" s="57"/>
+    </row>
+    <row r="52" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B52" s="57">
+      <c r="B52" s="56">
         <v>14</v>
       </c>
-      <c r="C52" s="64" t="s">
+      <c r="C52" s="63" t="s">
         <v>627</v>
       </c>
-      <c r="D52" s="64" t="s">
+      <c r="D52" s="63" t="s">
         <v>626</v>
       </c>
-      <c r="E52" s="57"/>
-      <c r="F52" s="58"/>
-      <c r="G52" s="58"/>
-    </row>
-    <row r="53" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="57" t="s">
+      <c r="E52" s="56"/>
+      <c r="F52" s="57"/>
+      <c r="G52" s="57"/>
+    </row>
+    <row r="53" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B53" s="57">
+      <c r="B53" s="56">
         <v>66</v>
       </c>
-      <c r="C53" s="66" t="s">
+      <c r="C53" s="65" t="s">
         <v>525</v>
       </c>
-      <c r="D53" s="62" t="s">
+      <c r="D53" s="61" t="s">
         <v>526</v>
       </c>
-      <c r="E53" s="57"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
-    </row>
-    <row r="54" spans="1:7" s="59" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="57" t="s">
+      <c r="E53" s="56"/>
+      <c r="F53" s="57"/>
+      <c r="G53" s="57"/>
+    </row>
+    <row r="54" spans="1:7" s="58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="56" t="s">
         <v>528</v>
       </c>
-      <c r="B54" s="57">
+      <c r="B54" s="56">
         <v>88</v>
       </c>
-      <c r="C54" s="66" t="s">
+      <c r="C54" s="65" t="s">
         <v>628</v>
       </c>
-      <c r="D54" s="62" t="s">
+      <c r="D54" s="61" t="s">
         <v>527</v>
       </c>
-      <c r="E54" s="57"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
+      <c r="E54" s="56"/>
+      <c r="F54" s="57"/>
+      <c r="G54" s="57"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="4"/>
@@ -4869,233 +4865,233 @@
       <c r="C56" s="5" t="s">
         <v>338</v>
       </c>
-      <c r="D56" s="42" t="s">
+      <c r="D56" s="41" t="s">
         <v>529</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="6"/>
       <c r="G56" s="6"/>
     </row>
-    <row r="57" spans="1:7" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="50" t="s">
+    <row r="57" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B57" s="50" t="s">
+      <c r="B57" s="49" t="s">
         <v>393</v>
       </c>
-      <c r="C57" s="52" t="s">
+      <c r="C57" s="51" t="s">
         <v>339</v>
       </c>
-      <c r="D57" s="51" t="s">
+      <c r="D57" s="50" t="s">
         <v>530</v>
       </c>
-      <c r="E57" s="52"/>
-      <c r="F57" s="53"/>
-      <c r="G57" s="53"/>
-    </row>
-    <row r="58" spans="1:7" s="54" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="50" t="s">
+      <c r="E57" s="51"/>
+      <c r="F57" s="52"/>
+      <c r="G57" s="52"/>
+    </row>
+    <row r="58" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B58" s="50" t="s">
+      <c r="B58" s="49" t="s">
         <v>394</v>
       </c>
-      <c r="C58" s="52" t="s">
+      <c r="C58" s="51" t="s">
         <v>340</v>
       </c>
-      <c r="D58" s="51" t="s">
+      <c r="D58" s="50" t="s">
         <v>531</v>
       </c>
-      <c r="E58" s="52"/>
-      <c r="F58" s="53"/>
-      <c r="G58" s="53"/>
-    </row>
-    <row r="59" spans="1:7" s="48" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A59" s="44" t="s">
+      <c r="E58" s="51"/>
+      <c r="F58" s="52"/>
+      <c r="G58" s="52"/>
+    </row>
+    <row r="59" spans="1:7" s="47" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B59" s="46" t="s">
+      <c r="B59" s="45" t="s">
         <v>532</v>
       </c>
-      <c r="C59" s="45" t="s">
+      <c r="C59" s="44" t="s">
         <v>533</v>
       </c>
-      <c r="D59" s="44" t="s">
+      <c r="D59" s="43" t="s">
         <v>534</v>
       </c>
-      <c r="E59" s="45"/>
-      <c r="F59" s="47"/>
-      <c r="G59" s="47"/>
-    </row>
-    <row r="60" spans="1:7" s="48" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A60" s="44" t="s">
+      <c r="E59" s="44"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+    </row>
+    <row r="60" spans="1:7" s="47" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B60" s="46" t="s">
+      <c r="B60" s="45" t="s">
         <v>535</v>
       </c>
-      <c r="C60" s="45" t="s">
+      <c r="C60" s="44" t="s">
         <v>536</v>
       </c>
-      <c r="D60" s="44" t="s">
+      <c r="D60" s="43" t="s">
         <v>537</v>
       </c>
-      <c r="E60" s="45"/>
-      <c r="F60" s="47"/>
-      <c r="G60" s="47"/>
-    </row>
-    <row r="61" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="44" t="s">
+      <c r="E60" s="44"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="46"/>
+    </row>
+    <row r="61" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B61" s="46" t="s">
+      <c r="B61" s="45" t="s">
         <v>538</v>
       </c>
-      <c r="C61" s="45" t="s">
+      <c r="C61" s="44" t="s">
         <v>539</v>
       </c>
-      <c r="D61" s="44" t="s">
+      <c r="D61" s="43" t="s">
         <v>540</v>
       </c>
-      <c r="E61" s="45"/>
-      <c r="F61" s="47"/>
-      <c r="G61" s="47"/>
-    </row>
-    <row r="62" spans="1:7" s="48" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="44" t="s">
+      <c r="E61" s="44"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="46"/>
+    </row>
+    <row r="62" spans="1:7" s="47" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B62" s="46" t="s">
+      <c r="B62" s="45" t="s">
         <v>541</v>
       </c>
-      <c r="C62" s="45" t="s">
+      <c r="C62" s="44" t="s">
         <v>542</v>
       </c>
-      <c r="D62" s="44" t="s">
+      <c r="D62" s="43" t="s">
         <v>543</v>
       </c>
-      <c r="E62" s="45"/>
-      <c r="F62" s="47"/>
-      <c r="G62" s="47"/>
-    </row>
-    <row r="63" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="44" t="s">
+      <c r="E62" s="44"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="46"/>
+    </row>
+    <row r="63" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B63" s="46" t="s">
+      <c r="B63" s="45" t="s">
         <v>544</v>
       </c>
-      <c r="C63" s="45" t="s">
+      <c r="C63" s="44" t="s">
         <v>545</v>
       </c>
-      <c r="D63" s="44" t="s">
+      <c r="D63" s="43" t="s">
         <v>546</v>
       </c>
-      <c r="E63" s="45"/>
-      <c r="F63" s="47"/>
-      <c r="G63" s="47"/>
-    </row>
-    <row r="64" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="44" t="s">
+      <c r="E63" s="44"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+    </row>
+    <row r="64" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B64" s="46" t="s">
+      <c r="B64" s="45" t="s">
         <v>547</v>
       </c>
-      <c r="C64" s="45" t="s">
+      <c r="C64" s="44" t="s">
         <v>548</v>
       </c>
-      <c r="D64" s="44" t="s">
+      <c r="D64" s="43" t="s">
         <v>549</v>
       </c>
-      <c r="E64" s="45"/>
-      <c r="F64" s="47"/>
-      <c r="G64" s="47"/>
-    </row>
-    <row r="65" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="44" t="s">
+      <c r="E64" s="44"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="46"/>
+    </row>
+    <row r="65" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B65" s="46" t="s">
+      <c r="B65" s="45" t="s">
         <v>550</v>
       </c>
-      <c r="C65" s="45" t="s">
+      <c r="C65" s="44" t="s">
         <v>551</v>
       </c>
-      <c r="D65" s="44" t="s">
+      <c r="D65" s="43" t="s">
         <v>552</v>
       </c>
-      <c r="E65" s="45"/>
-      <c r="F65" s="47"/>
-      <c r="G65" s="47"/>
-    </row>
-    <row r="66" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="44" t="s">
+      <c r="E65" s="44"/>
+      <c r="F65" s="46"/>
+      <c r="G65" s="46"/>
+    </row>
+    <row r="66" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B66" s="46" t="s">
+      <c r="B66" s="45" t="s">
         <v>553</v>
       </c>
-      <c r="C66" s="45" t="s">
+      <c r="C66" s="44" t="s">
         <v>554</v>
       </c>
-      <c r="D66" s="44" t="s">
+      <c r="D66" s="43" t="s">
         <v>555</v>
       </c>
-      <c r="E66" s="45"/>
-      <c r="F66" s="47"/>
-      <c r="G66" s="47"/>
-    </row>
-    <row r="67" spans="1:7" s="48" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A67" s="44" t="s">
+      <c r="E66" s="44"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+    </row>
+    <row r="67" spans="1:7" s="47" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B67" s="46" t="s">
+      <c r="B67" s="45" t="s">
         <v>556</v>
       </c>
-      <c r="C67" s="45" t="s">
+      <c r="C67" s="44" t="s">
         <v>557</v>
       </c>
-      <c r="D67" s="44" t="s">
+      <c r="D67" s="43" t="s">
         <v>558</v>
       </c>
-      <c r="E67" s="45"/>
-      <c r="F67" s="47"/>
-      <c r="G67" s="47"/>
-    </row>
-    <row r="68" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="44" t="s">
+      <c r="E67" s="44"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
+    </row>
+    <row r="68" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B68" s="46" t="s">
+      <c r="B68" s="45" t="s">
         <v>606</v>
       </c>
-      <c r="C68" s="45" t="s">
+      <c r="C68" s="44" t="s">
         <v>607</v>
       </c>
-      <c r="D68" s="44" t="s">
+      <c r="D68" s="43" t="s">
         <v>527</v>
       </c>
-      <c r="E68" s="45"/>
-      <c r="F68" s="47"/>
-      <c r="G68" s="47"/>
-    </row>
-    <row r="69" spans="1:7" s="48" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="44" t="s">
+      <c r="E68" s="44"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="46"/>
+    </row>
+    <row r="69" spans="1:7" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="B69" s="46" t="s">
+      <c r="B69" s="45" t="s">
         <v>559</v>
       </c>
-      <c r="C69" s="45" t="s">
+      <c r="C69" s="44" t="s">
         <v>560</v>
       </c>
-      <c r="D69" s="44" t="s">
+      <c r="D69" s="43" t="s">
         <v>561</v>
       </c>
-      <c r="E69" s="45"/>
-      <c r="F69" s="47"/>
-      <c r="G69" s="47"/>
+      <c r="E69" s="44"/>
+      <c r="F69" s="46"/>
+      <c r="G69" s="46"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
@@ -5110,13 +5106,13 @@
       <c r="A71" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B71" s="42" t="s">
+      <c r="B71" s="41" t="s">
         <v>637</v>
       </c>
-      <c r="C71" s="60" t="s">
+      <c r="C71" s="59" t="s">
         <v>388</v>
       </c>
-      <c r="D71" s="62" t="s">
+      <c r="D71" s="61" t="s">
         <v>562</v>
       </c>
       <c r="E71" s="5"/>
@@ -5127,13 +5123,13 @@
       <c r="A72" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B72" s="42" t="s">
+      <c r="B72" s="41" t="s">
         <v>638</v>
       </c>
-      <c r="C72" s="60" t="s">
+      <c r="C72" s="59" t="s">
         <v>389</v>
       </c>
-      <c r="D72" s="62" t="s">
+      <c r="D72" s="61" t="s">
         <v>563</v>
       </c>
       <c r="E72" s="5"/>
@@ -5144,13 +5140,13 @@
       <c r="A73" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B73" s="42" t="s">
+      <c r="B73" s="41" t="s">
         <v>639</v>
       </c>
-      <c r="C73" s="61" t="s">
+      <c r="C73" s="60" t="s">
         <v>645</v>
       </c>
-      <c r="D73" s="63" t="s">
+      <c r="D73" s="62" t="s">
         <v>645</v>
       </c>
       <c r="E73" s="5"/>
@@ -5195,13 +5191,13 @@
       <c r="A76" s="6" t="s">
         <v>564</v>
       </c>
-      <c r="B76" s="42" t="s">
+      <c r="B76" s="41" t="s">
         <v>639</v>
       </c>
-      <c r="C76" s="61" t="s">
+      <c r="C76" s="60" t="s">
         <v>645</v>
       </c>
-      <c r="D76" s="63" t="s">
+      <c r="D76" s="62" t="s">
         <v>645</v>
       </c>
       <c r="E76" s="5"/>
@@ -5235,7 +5231,7 @@
       <c r="C78" s="5" t="s">
         <v>342</v>
       </c>
-      <c r="D78" s="55" t="s">
+      <c r="D78" s="54" t="s">
         <v>566</v>
       </c>
       <c r="E78" s="5"/>
@@ -5252,7 +5248,7 @@
       <c r="C79" s="5" t="s">
         <v>343</v>
       </c>
-      <c r="D79" s="55" t="s">
+      <c r="D79" s="54" t="s">
         <v>567</v>
       </c>
       <c r="E79" s="5"/>
@@ -5269,7 +5265,7 @@
       <c r="C80" s="5" t="s">
         <v>344</v>
       </c>
-      <c r="D80" s="42" t="s">
+      <c r="D80" s="41" t="s">
         <v>568</v>
       </c>
       <c r="E80" s="5"/>
@@ -5286,7 +5282,7 @@
       <c r="C81" s="5" t="s">
         <v>345</v>
       </c>
-      <c r="D81" s="42" t="s">
+      <c r="D81" s="41" t="s">
         <v>569</v>
       </c>
       <c r="E81" s="5"/>
@@ -5320,7 +5316,7 @@
       <c r="C83" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="D83" s="42" t="s">
+      <c r="D83" s="41" t="s">
         <v>571</v>
       </c>
       <c r="E83" s="5"/>
@@ -5337,7 +5333,7 @@
       <c r="C84" s="5" t="s">
         <v>348</v>
       </c>
-      <c r="D84" s="42" t="s">
+      <c r="D84" s="41" t="s">
         <v>572</v>
       </c>
       <c r="E84" s="5"/>
@@ -5457,7 +5453,7 @@
       <c r="C92" s="7" t="s">
         <v>599</v>
       </c>
-      <c r="D92" s="64" t="s">
+      <c r="D92" s="63" t="s">
         <v>644</v>
       </c>
       <c r="E92" s="7"/>
@@ -5606,8 +5602,8 @@
       <c r="E103" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="F103" s="38"/>
-      <c r="G103" s="40"/>
+      <c r="F103" s="37"/>
+      <c r="G103" s="39"/>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="6" t="s">
@@ -5625,8 +5621,8 @@
       <c r="E104" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F104" s="38"/>
-      <c r="G104" s="40"/>
+      <c r="F104" s="37"/>
+      <c r="G104" s="39"/>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="6" t="s">
@@ -5644,8 +5640,8 @@
       <c r="E105" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F105" s="38"/>
-      <c r="G105" s="40"/>
+      <c r="F105" s="37"/>
+      <c r="G105" s="39"/>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="6" t="s">
@@ -5663,8 +5659,8 @@
       <c r="E106" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F106" s="38"/>
-      <c r="G106" s="40"/>
+      <c r="F106" s="37"/>
+      <c r="G106" s="39"/>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="6" t="s">
@@ -5682,8 +5678,8 @@
       <c r="E107" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="F107" s="38"/>
-      <c r="G107" s="40"/>
+      <c r="F107" s="37"/>
+      <c r="G107" s="39"/>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="6" t="s">
@@ -5701,8 +5697,8 @@
       <c r="E108" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="F108" s="38"/>
-      <c r="G108" s="40"/>
+      <c r="F108" s="37"/>
+      <c r="G108" s="39"/>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="6" t="s">
@@ -5720,8 +5716,8 @@
       <c r="E109" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="F109" s="38"/>
-      <c r="G109" s="40"/>
+      <c r="F109" s="37"/>
+      <c r="G109" s="39"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="6" t="s">
@@ -5739,8 +5735,8 @@
       <c r="E110" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F110" s="38"/>
-      <c r="G110" s="40"/>
+      <c r="F110" s="37"/>
+      <c r="G110" s="39"/>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
@@ -5758,8 +5754,8 @@
       <c r="E111" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F111" s="38"/>
-      <c r="G111" s="40"/>
+      <c r="F111" s="37"/>
+      <c r="G111" s="39"/>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="6" t="s">
@@ -5777,8 +5773,8 @@
       <c r="E112" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="F112" s="38"/>
-      <c r="G112" s="40"/>
+      <c r="F112" s="37"/>
+      <c r="G112" s="39"/>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="3"/>
@@ -5786,8 +5782,8 @@
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
-      <c r="F113" s="38"/>
-      <c r="G113" s="40"/>
+      <c r="F113" s="37"/>
+      <c r="G113" s="39"/>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="6" t="s">
@@ -5806,7 +5802,7 @@
       <c r="F114" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G114" s="40"/>
+      <c r="G114" s="39"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="6" t="s">
@@ -5825,7 +5821,7 @@
       <c r="F115" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G115" s="40"/>
+      <c r="G115" s="39"/>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="6" t="s">
@@ -5844,7 +5840,7 @@
       <c r="F116" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G116" s="40"/>
+      <c r="G116" s="39"/>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="6" t="s">
@@ -5863,7 +5859,7 @@
       <c r="F117" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G117" s="40"/>
+      <c r="G117" s="39"/>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="6" t="s">
@@ -5882,7 +5878,7 @@
       <c r="F118" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G118" s="40"/>
+      <c r="G118" s="39"/>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="6" t="s">
@@ -5901,7 +5897,7 @@
       <c r="F119" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G119" s="40"/>
+      <c r="G119" s="39"/>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="6" t="s">
@@ -5920,7 +5916,7 @@
       <c r="F120" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G120" s="40"/>
+      <c r="G120" s="39"/>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="6" t="s">
@@ -5939,7 +5935,7 @@
       <c r="F121" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G121" s="40"/>
+      <c r="G121" s="39"/>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="6" t="s">
@@ -5958,7 +5954,7 @@
       <c r="F122" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G122" s="40"/>
+      <c r="G122" s="39"/>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="6" t="s">
@@ -5977,7 +5973,7 @@
       <c r="F123" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="G123" s="40"/>
+      <c r="G123" s="39"/>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="6" t="s">
@@ -13930,8 +13926,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -13953,12 +13949,12 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>649</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>648</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>649</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>395</v>
@@ -16536,10 +16532,10 @@
       <c r="C71" s="19" t="s">
         <v>170</v>
       </c>
-      <c r="D71" s="34" t="s">
+      <c r="D71" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="E71" s="34" t="s">
+      <c r="E71" s="33" t="s">
         <v>367</v>
       </c>
       <c r="F71" s="19">
@@ -16764,10 +16760,10 @@
       <c r="O77" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="Q77" s="34" t="s">
+      <c r="Q77" s="33" t="s">
         <v>188</v>
       </c>
-      <c r="R77" s="34" t="s">
+      <c r="R77" s="33" t="s">
         <v>367</v>
       </c>
     </row>

</xml_diff>